<commit_message>
changing the annual bound on geological storage of co2 to 1Gt per year and region
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_UpdateGeologicalStorage.xlsx
+++ b/SuppXLS/Scen_UpdateGeologicalStorage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda_models\IEMM_v60_10-1\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF62716-2F00-4325-94E9-85EE68F3F5DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6203E60-C7E4-4C9F-8374-6F3BD04EC409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="23040" windowHeight="12072" xr2:uid="{A8DB3A7E-B09C-49B7-96A8-B31B03D81B01}"/>
+    <workbookView xWindow="3072" yWindow="3072" windowWidth="23040" windowHeight="12120" xr2:uid="{A8DB3A7E-B09C-49B7-96A8-B31B03D81B01}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -474,8 +474,7 @@
         <v>8</v>
       </c>
       <c r="P13">
-        <f>P12/10</f>
-        <v>600000000</v>
+        <v>1000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>